<commit_message>
Correción Revisión del uso de VS y CS
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-EncounterCL.xlsx
+++ b/output/StructureDefinition-EncounterCL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2817" uniqueCount="485">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-24T20:56:59-04:00</t>
+    <t>2024-06-25T09:03:09-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -705,10 +705,7 @@
     <t>example</t>
   </si>
   <si>
-    <t>The type of encounter.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/encounter-type</t>
+    <t>https://hl7chile.cl/fhir/ig/clcore/ValueSet/VSTiposEncuentroCL</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -729,10 +726,7 @@
     <t>Categorización del servicio que se va a prestar en el encuentro (por ejemplo, servicio de Ginecología)</t>
   </si>
   <si>
-    <t>Broad categorization of the service that is to be provided.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/service-type</t>
+    <t>https://hl7chile.cl/fhir/ig/clcore/ValueSet/VSTiposServicio</t>
   </si>
   <si>
     <t>PV1-10</t>
@@ -1882,7 +1876,7 @@
     <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="72.99609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="56.1875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.4453125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
@@ -4803,11 +4797,9 @@
       <c r="X26" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="Y26" t="s" s="2">
+      <c r="Y26" s="2"/>
+      <c r="Z26" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="Z26" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>81</v>
@@ -4840,24 +4832,24 @@
         <v>101</v>
       </c>
       <c r="AK26" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AL26" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>199</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4883,10 +4875,10 @@
         <v>216</v>
       </c>
       <c r="L27" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>228</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4915,11 +4907,9 @@
       <c r="X27" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>229</v>
-      </c>
+      <c r="Y27" s="2"/>
       <c r="Z27" t="s" s="2">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>81</v>
@@ -4937,7 +4927,7 @@
         <v>81</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>79</v>
@@ -4952,7 +4942,7 @@
         <v>101</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>170</v>
@@ -4961,15 +4951,15 @@
         <v>81</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4995,10 +4985,10 @@
         <v>216</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -5028,10 +5018,10 @@
         <v>220</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>81</v>
@@ -5049,7 +5039,7 @@
         <v>81</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
@@ -5067,25 +5057,25 @@
         <v>81</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="AM28" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AN28" t="s" s="2">
         <v>236</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="AN28" t="s" s="2">
-        <v>238</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -5104,16 +5094,16 @@
         <v>90</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="M29" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5163,7 +5153,7 @@
         <v>81</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>79</v>
@@ -5178,24 +5168,24 @@
         <v>101</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>248</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5218,13 +5208,13 @@
         <v>90</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>252</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5275,7 +5265,7 @@
         <v>81</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>79</v>
@@ -5290,28 +5280,28 @@
         <v>101</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>170</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -5330,13 +5320,13 @@
         <v>81</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5387,7 +5377,7 @@
         <v>81</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5402,10 +5392,10 @@
         <v>101</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>81</v>
@@ -5416,10 +5406,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5445,10 +5435,10 @@
         <v>166</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5499,7 +5489,7 @@
         <v>81</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -5514,24 +5504,24 @@
         <v>101</v>
       </c>
       <c r="AK32" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AM32" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AN32" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AN32" t="s" s="2">
-        <v>268</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5640,10 +5630,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5754,10 +5744,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5870,10 +5860,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5899,13 +5889,13 @@
         <v>216</v>
       </c>
       <c r="L36" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="N36" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -5935,7 +5925,7 @@
       </c>
       <c r="Y36" s="2"/>
       <c r="Z36" t="s" s="2">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>81</v>
@@ -5953,7 +5943,7 @@
         <v>81</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -5968,24 +5958,24 @@
         <v>101</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AM36" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AN36" t="s" s="2">
         <v>277</v>
-      </c>
-      <c r="AL36" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="AM36" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AN36" t="s" s="2">
-        <v>279</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6011,10 +6001,10 @@
         <v>190</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6065,7 +6055,7 @@
         <v>81</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6083,21 +6073,21 @@
         <v>81</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6120,13 +6110,13 @@
         <v>90</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6177,7 +6167,7 @@
         <v>81</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6192,24 +6182,24 @@
         <v>101</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AL38" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="AL38" t="s" s="2">
+      <c r="AN38" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="AM38" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="AN38" t="s" s="2">
-        <v>292</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6232,13 +6222,13 @@
         <v>90</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>296</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6289,7 +6279,7 @@
         <v>81</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6304,24 +6294,24 @@
         <v>101</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6347,13 +6337,13 @@
         <v>190</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6403,7 +6393,7 @@
         <v>81</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6418,24 +6408,24 @@
         <v>101</v>
       </c>
       <c r="AK40" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="AL40" t="s" s="2">
+      <c r="AN40" t="s" s="2">
         <v>303</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>305</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6544,10 +6534,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6617,16 +6607,16 @@
         <v>81</v>
       </c>
       <c r="AB42" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AE42" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>178</v>
@@ -6658,10 +6648,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6684,16 +6674,16 @@
         <v>90</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6743,7 +6733,7 @@
         <v>81</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6752,7 +6742,7 @@
         <v>89</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>101</v>
@@ -6761,21 +6751,21 @@
         <v>81</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6798,23 +6788,23 @@
         <v>90</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="N44" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q44" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="R44" t="s" s="2">
         <v>81</v>
@@ -6859,7 +6849,7 @@
         <v>81</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6868,7 +6858,7 @@
         <v>89</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>101</v>
@@ -6877,21 +6867,21 @@
         <v>81</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6914,16 +6904,16 @@
         <v>81</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="N45" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6973,7 +6963,7 @@
         <v>81</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -6988,28 +6978,28 @@
         <v>101</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7031,13 +7021,13 @@
         <v>216</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7066,10 +7056,10 @@
         <v>113</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>81</v>
@@ -7087,7 +7077,7 @@
         <v>81</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7102,28 +7092,28 @@
         <v>101</v>
       </c>
       <c r="AK46" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AL46" t="s" s="2">
+      <c r="AN46" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>343</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7142,16 +7132,16 @@
         <v>90</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L47" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>347</v>
-      </c>
       <c r="N47" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7201,7 +7191,7 @@
         <v>81</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7216,24 +7206,24 @@
         <v>101</v>
       </c>
       <c r="AK47" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AL47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>343</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7259,10 +7249,10 @@
         <v>166</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7313,7 +7303,7 @@
         <v>81</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7331,7 +7321,7 @@
         <v>81</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>81</v>
@@ -7342,10 +7332,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7454,10 +7444,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7568,10 +7558,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7684,14 +7674,14 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -7710,16 +7700,16 @@
         <v>90</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="L52" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>358</v>
-      </c>
       <c r="N52" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7769,7 +7759,7 @@
         <v>81</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>89</v>
@@ -7784,24 +7774,24 @@
         <v>101</v>
       </c>
       <c r="AK52" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AN52" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7827,10 +7817,10 @@
         <v>216</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -7860,10 +7850,10 @@
         <v>113</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Z53" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>81</v>
@@ -7881,7 +7871,7 @@
         <v>81</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>79</v>
@@ -7910,10 +7900,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7936,13 +7926,13 @@
         <v>81</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -7993,7 +7983,7 @@
         <v>81</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>79</v>
@@ -8011,7 +8001,7 @@
         <v>81</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>81</v>
@@ -8022,10 +8012,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8048,16 +8038,16 @@
         <v>81</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8107,7 +8097,7 @@
         <v>81</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>79</v>
@@ -8125,7 +8115,7 @@
         <v>81</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>81</v>
@@ -8136,10 +8126,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8165,13 +8155,13 @@
         <v>166</v>
       </c>
       <c r="L56" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="N56" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8221,7 +8211,7 @@
         <v>81</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>79</v>
@@ -8239,7 +8229,7 @@
         <v>81</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>81</v>
@@ -8250,10 +8240,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8362,10 +8352,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8476,10 +8466,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8592,10 +8582,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8621,10 +8611,10 @@
         <v>147</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8675,7 +8665,7 @@
         <v>81</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>79</v>
@@ -8699,15 +8689,15 @@
         <v>81</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8730,13 +8720,13 @@
         <v>81</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M61" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8787,7 +8777,7 @@
         <v>81</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -8805,7 +8795,7 @@
         <v>81</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>81</v>
@@ -8816,10 +8806,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8845,10 +8835,10 @@
         <v>216</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -8878,10 +8868,10 @@
         <v>113</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>81</v>
@@ -8899,7 +8889,7 @@
         <v>81</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -8917,21 +8907,21 @@
         <v>81</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -8957,10 +8947,10 @@
         <v>216</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -8990,10 +8980,10 @@
         <v>220</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>81</v>
@@ -9011,7 +9001,7 @@
         <v>81</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>79</v>
@@ -9035,15 +9025,15 @@
         <v>81</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9069,16 +9059,16 @@
         <v>216</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="N64" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="O64" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>411</v>
-      </c>
-      <c r="O64" t="s" s="2">
-        <v>412</v>
       </c>
       <c r="P64" t="s" s="2">
         <v>81</v>
@@ -9106,10 +9096,10 @@
         <v>220</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="Z64" t="s" s="2">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>81</v>
@@ -9127,7 +9117,7 @@
         <v>81</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>79</v>
@@ -9145,21 +9135,21 @@
         <v>81</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9185,10 +9175,10 @@
         <v>216</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -9218,10 +9208,10 @@
         <v>113</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="Z65" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AA65" t="s" s="2">
         <v>81</v>
@@ -9239,7 +9229,7 @@
         <v>81</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>79</v>
@@ -9257,21 +9247,21 @@
         <v>81</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9297,10 +9287,10 @@
         <v>216</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -9330,10 +9320,10 @@
         <v>113</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="Z66" t="s" s="2">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AA66" t="s" s="2">
         <v>81</v>
@@ -9351,7 +9341,7 @@
         <v>81</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>79</v>
@@ -9369,21 +9359,21 @@
         <v>81</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9406,13 +9396,13 @@
         <v>81</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -9463,7 +9453,7 @@
         <v>81</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>79</v>
@@ -9481,21 +9471,21 @@
         <v>81</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9521,10 +9511,10 @@
         <v>216</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -9554,10 +9544,10 @@
         <v>220</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="Z68" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AA68" t="s" s="2">
         <v>81</v>
@@ -9575,7 +9565,7 @@
         <v>81</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -9593,21 +9583,21 @@
         <v>81</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9633,13 +9623,13 @@
         <v>166</v>
       </c>
       <c r="L69" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="N69" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>446</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -9689,7 +9679,7 @@
         <v>81</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -9707,7 +9697,7 @@
         <v>81</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>81</v>
@@ -9718,10 +9708,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -9830,10 +9820,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -9944,10 +9934,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10060,10 +10050,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10086,13 +10076,13 @@
         <v>81</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>453</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>454</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10143,7 +10133,7 @@
         <v>81</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>89</v>
@@ -10158,24 +10148,24 @@
         <v>101</v>
       </c>
       <c r="AK73" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AM73" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="AN73" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>456</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>457</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10201,13 +10191,13 @@
         <v>109</v>
       </c>
       <c r="L74" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="M74" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="N74" t="s" s="2">
         <v>459</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>461</v>
       </c>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
@@ -10236,10 +10226,10 @@
         <v>158</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>81</v>
@@ -10257,7 +10247,7 @@
         <v>81</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
@@ -10275,7 +10265,7 @@
         <v>81</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>81</v>
@@ -10286,10 +10276,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10315,13 +10305,13 @@
         <v>216</v>
       </c>
       <c r="L75" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="N75" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
@@ -10350,10 +10340,10 @@
         <v>220</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z75" t="s" s="2">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AA75" t="s" s="2">
         <v>81</v>
@@ -10371,7 +10361,7 @@
         <v>81</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -10400,10 +10390,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10429,10 +10419,10 @@
         <v>190</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -10483,7 +10473,7 @@
         <v>81</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
@@ -10501,7 +10491,7 @@
         <v>81</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>81</v>
@@ -10512,10 +10502,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10538,13 +10528,13 @@
         <v>81</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="L77" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="M77" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -10595,7 +10585,7 @@
         <v>81</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>79</v>
@@ -10610,24 +10600,24 @@
         <v>101</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -10650,16 +10640,16 @@
         <v>81</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="L78" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="M78" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="L78" t="s" s="2">
+      <c r="N78" t="s" s="2">
         <v>482</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>483</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>484</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -10709,7 +10699,7 @@
         <v>81</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>79</v>
@@ -10724,10 +10714,10 @@
         <v>101</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>81</v>

</xml_diff>